<commit_message>
update mel to wav conversion
</commit_message>
<xml_diff>
--- a/research/audio_calculation.xlsx
+++ b/research/audio_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Programs\Poissound_flow\research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA01E3A2-5CA3-49EC-8689-2EE9AB8A191E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3975A357-3D78-49B9-8CFD-C9773B68A934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0A1E03ED-8DD3-4AE6-AE43-760BDE4590A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A1E03ED-8DD3-4AE6-AE43-760BDE4590A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>sr</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>freq resolution</t>
   </si>
 </sst>
 </file>
@@ -155,16 +158,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% - Accent3" xfId="2" builtinId="40"/>
@@ -481,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{195C0F66-BB62-4057-AB49-99CBB0EDE7B5}">
-  <dimension ref="C3:P5"/>
+  <dimension ref="C3:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,105 +503,154 @@
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" customWidth="1"/>
+    <col min="9" max="13" width="13.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="3" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L4" t="s">
+      <c r="J4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="P4" t="s">
         <v>9</v>
       </c>
-      <c r="M4" t="s">
+      <c r="Q4" t="s">
         <v>10</v>
       </c>
-      <c r="N4" t="s">
+      <c r="R4" t="s">
         <v>12</v>
       </c>
-      <c r="O4" t="s">
+      <c r="S4" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="T4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="2">
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>16000</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <f>G5*4</f>
         <v>1024</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>64</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>256</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <f>E5/D5 * 1000</f>
         <v>64</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <f>C5*D5/G5 + 1</f>
         <v>63.5</v>
       </c>
-      <c r="L5">
+      <c r="J5" s="1">
+        <f>D5/(2*F5)</f>
+        <v>125</v>
+      </c>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="P5">
         <v>900</v>
       </c>
-      <c r="M5">
+      <c r="Q5">
         <f>F5*(INT(I5)+1)</f>
         <v>4096</v>
       </c>
-      <c r="N5">
+      <c r="R5">
         <v>0.03</v>
       </c>
-      <c r="O5">
+      <c r="S5">
         <v>0.01</v>
       </c>
-      <c r="P5">
-        <f>0.75*(LN(L5/(2*SQRT(M5)*O5*O5)))/(LN(1+N5))</f>
+      <c r="T5">
+        <f>0.75*(LN(P5/(2*SQRT(Q5)*S5*S5)))/(LN(1+R5))</f>
         <v>283.18226784477122</v>
       </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>16000</v>
+      </c>
+      <c r="E6" s="1">
+        <v>512</v>
+      </c>
+      <c r="F6" s="1">
+        <v>128</v>
+      </c>
+      <c r="G6" s="1">
+        <v>128</v>
+      </c>
+      <c r="H6" s="1">
+        <f>E6/D6 * 1000</f>
+        <v>32</v>
+      </c>
+      <c r="I6" s="1">
+        <f>C6*D6/G6 + 1</f>
+        <v>126</v>
+      </c>
+      <c r="J6" s="1">
+        <f>D6/(2*F6)</f>
+        <v>62.5</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>